<commit_message>
Update all changes 1/16/2024 4:33 pm
</commit_message>
<xml_diff>
--- a/CASUAL/LA SP-VMO/DE SAGUN, NANCY.xlsx
+++ b/CASUAL/LA SP-VMO/DE SAGUN, NANCY.xlsx
@@ -27,7 +27,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'2017 LEAVE BALANCE'!$1:$9</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'2018 LEAVE CREDITS'!$1:$9</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="105">
   <si>
     <t>PERIOD</t>
   </si>
@@ -339,34 +339,13 @@
     <t>UT(0-1-52)</t>
   </si>
   <si>
-    <t>A(1-0-0)</t>
-  </si>
-  <si>
     <t>UT(0-1-17)</t>
   </si>
   <si>
-    <t>A(2-0-0)</t>
-  </si>
-  <si>
-    <t>6/23,24/2022</t>
-  </si>
-  <si>
     <t>UT(0-4-27)</t>
   </si>
   <si>
     <t>UT(0-0-15)</t>
-  </si>
-  <si>
-    <t>A(19-0-0)</t>
-  </si>
-  <si>
-    <t>4/1,4-8,11-13,18-22,25-29/2022</t>
-  </si>
-  <si>
-    <t>A(4-0-0)</t>
-  </si>
-  <si>
-    <t>5/2,4-6/2022</t>
   </si>
   <si>
     <t>UT(0-2-50)</t>
@@ -757,17 +736,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -777,6 +753,9 @@
     </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1307,7 +1286,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1350,7 +1329,7 @@
         <xdr:cNvPr id="5" name="TextBox 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1414,7 +1393,7 @@
         <xdr:cNvPr id="4" name="Arrow: Left 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1474,7 +1453,7 @@
         <xdr:cNvPr id="8" name="Oval 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1540,7 +1519,7 @@
         <xdr:cNvPr id="9" name="Arrow: Left-Right 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1603,7 +1582,7 @@
         <xdr:cNvPr id="10" name="TextBox 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1701,7 +1680,7 @@
         <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1760,7 +1739,7 @@
         <xdr:cNvPr id="19" name="TextBox 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1825,7 +1804,7 @@
         <xdr:cNvPr id="20" name="Picture 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1868,7 +1847,7 @@
         <xdr:cNvPr id="21" name="TextBox 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1943,7 +1922,7 @@
         <xdr:cNvPr id="22" name="TextBox 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2129,7 +2108,7 @@
         <xdr:cNvPr id="23" name="Oval 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2195,7 +2174,7 @@
         <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2253,7 +2232,7 @@
         <xdr:cNvPr id="26" name="Oval 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2319,7 +2298,7 @@
         <xdr:cNvPr id="27" name="Straight Arrow Connector 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2375,7 +2354,7 @@
         <xdr:cNvPr id="30" name="TextBox 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2450,7 +2429,7 @@
         <xdr:cNvPr id="31" name="Picture 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2493,7 +2472,7 @@
         <xdr:cNvPr id="32" name="Oval 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2559,7 +2538,7 @@
         <xdr:cNvPr id="33" name="Straight Arrow Connector 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2615,7 +2594,7 @@
         <xdr:cNvPr id="34" name="TextBox 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3091,9 +3070,9 @@
   <dimension ref="A2:M137"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3690" topLeftCell="A65" activePane="bottomLeft"/>
+      <pane ySplit="3690" topLeftCell="A68" activePane="bottomLeft"/>
       <selection activeCell="M9" sqref="M9"/>
-      <selection pane="bottomLeft" activeCell="O68" sqref="O68"/>
+      <selection pane="bottomLeft" activeCell="K87" sqref="K87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3123,14 +3102,14 @@
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="53"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -3141,14 +3120,14 @@
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="55"/>
-      <c r="G3" s="51"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="52"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="57"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="56"/>
     </row>
     <row r="4" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
@@ -3161,16 +3140,16 @@
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="51" t="s">
+      <c r="F4" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="G4" s="51"/>
+      <c r="G4" s="52"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="52"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="53"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
@@ -3196,18 +3175,18 @@
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53" t="s">
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="57"/>
       <c r="K7" s="14"/>
     </row>
     <row r="8" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -3254,7 +3233,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="13">
         <f>SUM(Table13[EARNED])-SUM(Table13[Absence Undertime W/ Pay])</f>
-        <v>10.456000000000017</v>
+        <v>36.456000000000017</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="13" t="str">
@@ -3305,7 +3284,7 @@
       <c r="D11" s="39"/>
       <c r="E11" s="9">
         <f>SUM(Table13[EARNED])-SUM(Table13[Absence Undertime W/ Pay])+CONVERTION!$A$3</f>
-        <v>26.081000000000017</v>
+        <v>52.081000000000017</v>
       </c>
       <c r="F11" s="20"/>
       <c r="G11" s="13">
@@ -4636,7 +4615,7 @@
         <v>44621</v>
       </c>
       <c r="B73" s="20" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C73" s="13">
         <v>1.25</v>
@@ -4659,15 +4638,11 @@
       <c r="A74" s="40">
         <v>44652</v>
       </c>
-      <c r="B74" s="20" t="s">
-        <v>106</v>
-      </c>
+      <c r="B74" s="20"/>
       <c r="C74" s="13">
         <v>1.25</v>
       </c>
-      <c r="D74" s="39">
-        <v>19</v>
-      </c>
+      <c r="D74" s="39"/>
       <c r="E74" s="9"/>
       <c r="F74" s="20"/>
       <c r="G74" s="13">
@@ -4677,23 +4652,17 @@
       <c r="H74" s="39"/>
       <c r="I74" s="9"/>
       <c r="J74" s="11"/>
-      <c r="K74" s="20" t="s">
-        <v>107</v>
-      </c>
+      <c r="K74" s="20"/>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="40">
         <v>44682</v>
       </c>
-      <c r="B75" s="20" t="s">
-        <v>108</v>
-      </c>
+      <c r="B75" s="20"/>
       <c r="C75" s="13">
         <v>1.25</v>
       </c>
-      <c r="D75" s="39">
-        <v>4</v>
-      </c>
+      <c r="D75" s="39"/>
       <c r="E75" s="9"/>
       <c r="F75" s="20"/>
       <c r="G75" s="13">
@@ -4703,14 +4672,12 @@
       <c r="H75" s="39"/>
       <c r="I75" s="9"/>
       <c r="J75" s="11"/>
-      <c r="K75" s="20" t="s">
-        <v>109</v>
-      </c>
+      <c r="K75" s="20"/>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="40"/>
       <c r="B76" s="20" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C76" s="13"/>
       <c r="D76" s="39">
@@ -4731,15 +4698,11 @@
       <c r="A77" s="40">
         <v>44713</v>
       </c>
-      <c r="B77" s="20" t="s">
-        <v>102</v>
-      </c>
+      <c r="B77" s="20"/>
       <c r="C77" s="13">
         <v>1.25</v>
       </c>
-      <c r="D77" s="39">
-        <v>2</v>
-      </c>
+      <c r="D77" s="39"/>
       <c r="E77" s="9"/>
       <c r="F77" s="20"/>
       <c r="G77" s="13">
@@ -4749,14 +4712,12 @@
       <c r="H77" s="39"/>
       <c r="I77" s="9"/>
       <c r="J77" s="11"/>
-      <c r="K77" s="20" t="s">
-        <v>103</v>
-      </c>
+      <c r="K77" s="20"/>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="40"/>
       <c r="B78" s="20" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C78" s="13"/>
       <c r="D78" s="39">
@@ -4777,15 +4738,11 @@
       <c r="A79" s="40">
         <v>44743</v>
       </c>
-      <c r="B79" s="20" t="s">
-        <v>100</v>
-      </c>
+      <c r="B79" s="20"/>
       <c r="C79" s="13">
         <v>1.25</v>
       </c>
-      <c r="D79" s="39">
-        <v>1</v>
-      </c>
+      <c r="D79" s="39"/>
       <c r="E79" s="9"/>
       <c r="F79" s="20"/>
       <c r="G79" s="13">
@@ -4795,14 +4752,12 @@
       <c r="H79" s="39"/>
       <c r="I79" s="9"/>
       <c r="J79" s="11"/>
-      <c r="K79" s="49">
-        <v>44755</v>
-      </c>
+      <c r="K79" s="49"/>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="40"/>
       <c r="B80" s="20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C80" s="13"/>
       <c r="D80" s="39">
@@ -4977,9 +4932,7 @@
       <c r="H87" s="39"/>
       <c r="I87" s="9"/>
       <c r="J87" s="11"/>
-      <c r="K87" s="49">
-        <v>44908</v>
-      </c>
+      <c r="K87" s="49"/>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="40"/>
@@ -5423,7 +5376,7 @@
       <c r="I106" s="9"/>
       <c r="J106" s="11"/>
       <c r="K106" s="20" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.25">
@@ -5932,17 +5885,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:J7"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="J3:K3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:J7"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
@@ -6010,14 +5963,14 @@
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="53"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -6030,14 +5983,14 @@
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="55"/>
-      <c r="G3" s="51"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="52"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="57"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="56"/>
     </row>
     <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
@@ -6050,16 +6003,16 @@
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="51" t="s">
+      <c r="F4" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="G4" s="51"/>
+      <c r="G4" s="52"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="52"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="53"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
@@ -6085,18 +6038,18 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53" t="s">
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="57"/>
       <c r="K7" s="14"/>
     </row>
     <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">

</xml_diff>